<commit_message>
-Added Yamaha YV100X SMT cordinat generate file feature.
</commit_message>
<xml_diff>
--- a/TestBOM.xlsx
+++ b/TestBOM.xlsx
@@ -2,23 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="585" windowWidth="27660" windowHeight="11955"/>
+    <workbookView xWindow="600" yWindow="780" windowWidth="23100" windowHeight="9120"/>
   </bookViews>
   <sheets>
-    <sheet name="Bill of Materials-SCH_PowerBoar" sheetId="1" r:id="rId1"/>
+    <sheet name="Bill of Materials-Project" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Print_Titles" localSheetId="0">'Bill of Materials-SCH_PowerBoar'!$1:$1</definedName>
+    <definedName name="Print_Titles" localSheetId="0">'Bill of Materials-Project'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Quantity</t>
   </si>
@@ -26,73 +27,97 @@
     <t>Designator</t>
   </si>
   <si>
-    <t>130000003</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>130000004</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>130000005</t>
-  </si>
-  <si>
-    <t>JK1</t>
-  </si>
-  <si>
-    <t>130000006</t>
-  </si>
-  <si>
-    <t>R9, R10, R11, R12, R13, R14, R15, R16, R17</t>
-  </si>
-  <si>
-    <t>130000007</t>
-  </si>
-  <si>
-    <t>P1, P4</t>
-  </si>
-  <si>
-    <t>130000008</t>
-  </si>
-  <si>
-    <t>RL3, RL6, RL9</t>
-  </si>
-  <si>
-    <t>130000009</t>
-  </si>
-  <si>
-    <t>P7, P19</t>
-  </si>
-  <si>
-    <t>130000010</t>
-  </si>
-  <si>
-    <t>P12, P20</t>
-  </si>
-  <si>
-    <t>130000011</t>
-  </si>
-  <si>
-    <t>P14, P18</t>
-  </si>
-  <si>
-    <t>130000012</t>
-  </si>
-  <si>
-    <t>U1, U4</t>
-  </si>
-  <si>
-    <t>130000013</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>Comp. No</t>
+    <t>CN4, CN5</t>
+  </si>
+  <si>
+    <t>130100001</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>130100008</t>
+  </si>
+  <si>
+    <t>CN1, CN2, CN3</t>
+  </si>
+  <si>
+    <t>130100009</t>
+  </si>
+  <si>
+    <t>J1, J3, J4, J5, J6, J7, J8, J9, J11, J12, J15, J16</t>
+  </si>
+  <si>
+    <t>130100010</t>
+  </si>
+  <si>
+    <t>130100011</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R6, R7, R8, R13, R20</t>
+  </si>
+  <si>
+    <t>130100016</t>
+  </si>
+  <si>
+    <t>U7, U8</t>
+  </si>
+  <si>
+    <t>130100014</t>
+  </si>
+  <si>
+    <t>C3, C5, C7, C9</t>
+  </si>
+  <si>
+    <t>130100005</t>
+  </si>
+  <si>
+    <t>C1, C2, C4</t>
+  </si>
+  <si>
+    <t>130100015</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>130100012</t>
+  </si>
+  <si>
+    <t>L1, L2, L3, L4, L5</t>
+  </si>
+  <si>
+    <t>130100006</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>130100003</t>
+  </si>
+  <si>
+    <t>LED3, LED4, LED5, LED6</t>
+  </si>
+  <si>
+    <t>130100004</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>130100007</t>
+  </si>
+  <si>
+    <t>U1, U3, U4, U5</t>
+  </si>
+  <si>
+    <t>KEY1, KEY2, KEY3, KEY4, KEY5, KEY6, KEY7, KEY8, KEY9, KEY10, KEY11, KEY12, KEY13, KEY14</t>
+  </si>
+  <si>
+    <t>R4, R5, R9, R10, R11, R12, R14, R25, R27, R28, R29, R30, R31, R32, R33</t>
+  </si>
+  <si>
+    <t>Erp Code</t>
   </si>
 </sst>
 </file>
@@ -103,10 +128,9 @@
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
-      <charset val="162"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,13 +138,16 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor rgb="FFD3D3D3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -129,6 +156,19 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -148,9 +188,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -180,25 +218,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -206,75 +269,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00E3E3E3"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0"/>
 </styleSheet>
 </file>
 
@@ -566,22 +561,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -591,131 +584,181 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="27" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="7">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C9" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="27" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
+      <c r="C13" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="27" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="40.5" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="27" customHeight="1">
+      <c r="A17" s="9"/>
+      <c r="B17" s="7">
         <v>14</v>
       </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
+      <c r="C17" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" blackAndWhite="1"/>
-  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
@@ -733,6 +776,22 @@
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" blackAndWhite="1"/>
-  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" blackAndWhite="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Some bug fixed and upgraded.
</commit_message>
<xml_diff>
--- a/TestBOM.xlsx
+++ b/TestBOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Quantity</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>Erp Code</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>130100099</t>
+  </si>
+  <si>
+    <t>130100098</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>130100097</t>
   </si>
 </sst>
 </file>
@@ -561,9 +579,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
@@ -735,23 +755,56 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="40.5" customHeight="1">
+    <row r="16" spans="1:3" ht="27" customHeight="1">
       <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="27" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="27" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="40.5" customHeight="1">
+      <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B19" s="7">
         <v>4</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="27" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="7">
+    <row r="20" spans="1:3" ht="27" customHeight="1">
+      <c r="A20" s="9"/>
+      <c r="B20" s="7">
         <v>14</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>